<commit_message>
changed amp to &
</commit_message>
<xml_diff>
--- a/MajorCrosswalk.xlsx
+++ b/MajorCrosswalk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\apfile.osg.ufl.edu\ap-aac$\AAC\AAC Tech\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsy\Documents\GitHub\Data-Warehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -329,9 +329,6 @@
     <t>ENE</t>
   </si>
   <si>
-    <t>Environmental Management in Agriculture &amp;amp; Natural Resources</t>
-  </si>
-  <si>
     <t>IS</t>
   </si>
   <si>
@@ -680,9 +677,6 @@
     <t>PSY</t>
   </si>
   <si>
-    <t>Psychology-Behavioral &amp;amp; Cognitive Neuroscience</t>
-  </si>
-  <si>
     <t>PBC</t>
   </si>
   <si>
@@ -1263,6 +1257,12 @@
   </si>
   <si>
     <t>College of Education</t>
+  </si>
+  <si>
+    <t>Environmental Management in Agriculture &amp; Natural Resources</t>
+  </si>
+  <si>
+    <t>Psychology-Behavioral &amp;  Cognitive Neuroscience</t>
   </si>
 </sst>
 </file>
@@ -1676,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="65.42578125" defaultRowHeight="15"/>
@@ -1691,27 +1691,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1723,15 +1723,15 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -1743,15 +1743,15 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -1763,15 +1763,15 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -1783,15 +1783,15 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>41</v>
@@ -1803,15 +1803,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>47</v>
@@ -1823,15 +1823,15 @@
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>77</v>
@@ -1843,15 +1843,15 @@
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>77</v>
@@ -1863,15 +1863,15 @@
         <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>96</v>
@@ -1883,315 +1883,315 @@
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
@@ -2203,75 +2203,75 @@
         <v>25</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>51</v>
@@ -2283,95 +2283,95 @@
         <v>53</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>70</v>
@@ -2383,15 +2383,15 @@
         <v>72</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>85</v>
@@ -2403,15 +2403,15 @@
         <v>87</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>88</v>
@@ -2423,15 +2423,15 @@
         <v>87</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>90</v>
@@ -2443,15 +2443,15 @@
         <v>87</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -2463,15 +2463,15 @@
         <v>7</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
@@ -2483,15 +2483,15 @@
         <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>54</v>
@@ -2503,15 +2503,15 @@
         <v>7</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>58</v>
@@ -2523,15 +2523,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>65</v>
@@ -2543,15 +2543,15 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>67</v>
@@ -2563,15 +2563,15 @@
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>79</v>
@@ -2583,15 +2583,15 @@
         <v>7</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>92</v>
@@ -2603,15 +2603,15 @@
         <v>7</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>98</v>
@@ -2623,155 +2623,155 @@
         <v>7</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>26</v>
@@ -2783,15 +2783,15 @@
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>29</v>
@@ -2803,15 +2803,15 @@
         <v>28</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>31</v>
@@ -2823,15 +2823,15 @@
         <v>28</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>75</v>
@@ -2843,15 +2843,15 @@
         <v>28</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>81</v>
@@ -2863,155 +2863,155 @@
         <v>28</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>20</v>
@@ -3023,75 +3023,75 @@
         <v>22</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>62</v>
@@ -3103,75 +3103,75 @@
         <v>64</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>2</v>
@@ -3183,18 +3183,18 @@
         <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>4</v>
@@ -3203,55 +3203,55 @@
         <v>4</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>8</v>
@@ -3263,15 +3263,15 @@
         <v>10</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>18</v>
@@ -3283,15 +3283,15 @@
         <v>10</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>33</v>
@@ -3303,15 +3303,15 @@
         <v>10</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>35</v>
@@ -3323,15 +3323,15 @@
         <v>10</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>37</v>
@@ -3343,15 +3343,15 @@
         <v>10</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>37</v>
@@ -3363,15 +3363,15 @@
         <v>10</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>37</v>
@@ -3383,15 +3383,15 @@
         <v>10</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>43</v>
@@ -3403,15 +3403,15 @@
         <v>10</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>45</v>
@@ -3423,15 +3423,15 @@
         <v>10</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>49</v>
@@ -3443,15 +3443,15 @@
         <v>10</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>56</v>
@@ -3463,15 +3463,15 @@
         <v>10</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>60</v>
@@ -3483,15 +3483,15 @@
         <v>10</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>67</v>
@@ -3503,15 +3503,15 @@
         <v>10</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>73</v>
@@ -3523,15 +3523,15 @@
         <v>10</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>83</v>
@@ -3543,15 +3543,15 @@
         <v>10</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>94</v>
@@ -3563,788 +3563,788 @@
         <v>10</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="D95" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="D96" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="D97" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="D98" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="D99" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="D100" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="D101" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="D102" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D103" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="D104" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="D105" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D106" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D107" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="D108" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="D109" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="D110" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="D111" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="D112" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="D113" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="D114" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="D115" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="D116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="D117" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="D118" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="D119" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>217</v>
+        <v>411</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="15.75" thickBot="1">
       <c r="A130" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="15.75" thickBot="1">
       <c r="A131" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B131" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C131" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="D131" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D131" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="E131" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F131" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="15.75" thickBot="1">
       <c r="A132" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B132" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C132" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="D132" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D132" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="E132" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F132" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="15.75" thickBot="1">
       <c r="A133" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B133" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="D133" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D133" s="4" t="s">
-        <v>214</v>
-      </c>
       <c r="E133" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F133" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>